<commit_message>
GOt the generic function working I think.
</commit_message>
<xml_diff>
--- a/Documents/Logic For Screenplay Reader.xlsx
+++ b/Documents/Logic For Screenplay Reader.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LOGIC of First Attempt" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>if Start of Script is True</t>
   </si>
@@ -135,6 +136,36 @@
   </si>
   <si>
     <t>return script_df</t>
+  </si>
+  <si>
+    <t>SCENE</t>
+  </si>
+  <si>
+    <t>CHARACTER</t>
+  </si>
+  <si>
+    <t>PARENTH</t>
+  </si>
+  <si>
+    <t>BLANK_LINE</t>
+  </si>
+  <si>
+    <t>CUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMERA DIRECTION </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSISTION </t>
+  </si>
+  <si>
+    <t>PAGE_NUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTINUED_PAGE </t>
+  </si>
+  <si>
+    <t>Determine with REgWhy</t>
   </si>
 </sst>
 </file>
@@ -454,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,6 +532,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
@@ -535,82 +569,88 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
       <c r="E17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
       <c r="F28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
         <v>13</v>
       </c>
@@ -703,6 +743,66 @@
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>